<commit_message>
created list of wearables
</commit_message>
<xml_diff>
--- a/references/utx000ext_timelines.xlsx
+++ b/references/utx000ext_timelines.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hagenfritz/Projects/utx000/references/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB599647-9D96-9149-AECF-FD6D4F72BDE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90E6875-05F9-9D45-BFA2-BC7B1A6FF109}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{A42CCD86-71DD-4C4D-87F8-705DB24E1636}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="76">
   <si>
     <t>Event 1</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>Phase 3 Reopening</t>
+  </si>
+  <si>
+    <t>Short Relocation Survey</t>
   </si>
 </sst>
 </file>
@@ -625,33 +628,6 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -676,16 +652,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1002,11 +1005,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D07724-71E6-3C40-BDBC-6CE123708DF5}">
-  <dimension ref="A1:GU43"/>
+  <dimension ref="A1:GZ43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="EW1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="FH5" sqref="FH5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="GL1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="GQ7" sqref="GQ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1015,9 +1018,9 @@
     <col min="33" max="33" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:203" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:203" x14ac:dyDescent="0.2">
-      <c r="B2" s="56" t="s">
+    <row r="1" spans="1:208" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:208" x14ac:dyDescent="0.2">
+      <c r="B2" s="62" t="s">
         <v>48</v>
       </c>
       <c r="C2" s="33"/>
@@ -1060,8 +1063,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:203" x14ac:dyDescent="0.2">
-      <c r="B3" s="56"/>
+    <row r="3" spans="1:208" x14ac:dyDescent="0.2">
+      <c r="B3" s="62"/>
       <c r="C3" s="33"/>
       <c r="D3" s="33"/>
       <c r="E3" s="33"/>
@@ -1099,8 +1102,8 @@
       <c r="DC3" s="3"/>
       <c r="FJ3" s="1"/>
     </row>
-    <row r="4" spans="1:203" x14ac:dyDescent="0.2">
-      <c r="B4" s="56"/>
+    <row r="4" spans="1:208" x14ac:dyDescent="0.2">
+      <c r="B4" s="62"/>
       <c r="C4" s="33"/>
       <c r="D4" s="33"/>
       <c r="E4" s="33"/>
@@ -1146,8 +1149,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:203" x14ac:dyDescent="0.2">
-      <c r="B5" s="56"/>
+    <row r="5" spans="1:208" x14ac:dyDescent="0.2">
+      <c r="B5" s="62"/>
       <c r="C5" s="33"/>
       <c r="D5" s="33"/>
       <c r="E5" s="33"/>
@@ -1189,22 +1192,22 @@
       </c>
       <c r="FJ5" s="1"/>
     </row>
-    <row r="6" spans="1:203" x14ac:dyDescent="0.2">
-      <c r="B6" s="56"/>
-      <c r="C6" s="68" t="s">
+    <row r="6" spans="1:208" x14ac:dyDescent="0.2">
+      <c r="B6" s="62"/>
+      <c r="C6" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="68"/>
-      <c r="E6" s="68"/>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="68"/>
-      <c r="I6" s="68"/>
-      <c r="J6" s="68"/>
-      <c r="K6" s="68"/>
-      <c r="L6" s="68"/>
-      <c r="M6" s="68"/>
-      <c r="N6" s="68"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+      <c r="G6" s="65"/>
+      <c r="H6" s="65"/>
+      <c r="I6" s="65"/>
+      <c r="J6" s="65"/>
+      <c r="K6" s="65"/>
+      <c r="L6" s="65"/>
+      <c r="M6" s="65"/>
+      <c r="N6" s="65"/>
       <c r="O6" s="33"/>
       <c r="P6" s="33"/>
       <c r="Q6" s="33"/>
@@ -1246,9 +1249,12 @@
         <v>8</v>
       </c>
       <c r="FJ6" s="1"/>
+      <c r="GY6" s="6" t="s">
+        <v>75</v>
+      </c>
     </row>
-    <row r="7" spans="1:203" x14ac:dyDescent="0.2">
-      <c r="B7" s="56"/>
+    <row r="7" spans="1:208" x14ac:dyDescent="0.2">
+      <c r="B7" s="62"/>
       <c r="C7" s="33"/>
       <c r="D7" s="33"/>
       <c r="E7" s="33"/>
@@ -1289,11 +1295,11 @@
       <c r="EM7" s="1"/>
       <c r="FJ7" s="1"/>
     </row>
-    <row r="8" spans="1:203" x14ac:dyDescent="0.2">
-      <c r="A8" s="60" t="s">
+    <row r="8" spans="1:208" x14ac:dyDescent="0.2">
+      <c r="A8" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="61"/>
+      <c r="B8" s="52"/>
       <c r="C8" s="16">
         <v>43843</v>
       </c>
@@ -1897,8 +1903,23 @@
       <c r="GU8" s="17">
         <v>44043</v>
       </c>
+      <c r="GV8" s="17">
+        <v>44044</v>
+      </c>
+      <c r="GW8" s="17">
+        <v>44045</v>
+      </c>
+      <c r="GX8" s="17">
+        <v>44046</v>
+      </c>
+      <c r="GY8" s="17">
+        <v>44047</v>
+      </c>
+      <c r="GZ8" s="17">
+        <v>44048</v>
+      </c>
     </row>
-    <row r="9" spans="1:203" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:208" x14ac:dyDescent="0.2">
       <c r="B9" s="9" t="s">
         <v>17</v>
       </c>
@@ -1936,17 +1957,17 @@
       <c r="AH9" s="9"/>
       <c r="BM9" s="1"/>
       <c r="BU9" s="25"/>
-      <c r="DA9" s="63" t="s">
+      <c r="DA9" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="DB9" s="63"/>
-      <c r="DC9" s="63"/>
-      <c r="DD9" s="63"/>
-      <c r="DE9" s="63"/>
-      <c r="DF9" s="63"/>
-      <c r="DG9" s="63"/>
-      <c r="DH9" s="63"/>
-      <c r="DI9" s="63"/>
+      <c r="DB9" s="54"/>
+      <c r="DC9" s="54"/>
+      <c r="DD9" s="54"/>
+      <c r="DE9" s="54"/>
+      <c r="DF9" s="54"/>
+      <c r="DG9" s="54"/>
+      <c r="DH9" s="54"/>
+      <c r="DI9" s="54"/>
       <c r="DL9" s="1"/>
       <c r="DO9" s="1"/>
       <c r="EA9" s="1"/>
@@ -1954,7 +1975,7 @@
       <c r="FA9" s="1"/>
       <c r="FH9" s="1"/>
     </row>
-    <row r="10" spans="1:203" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:208" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
         <v>22</v>
       </c>
@@ -2001,8 +2022,11 @@
       <c r="EJ10" s="1"/>
       <c r="FA10" s="1"/>
       <c r="FH10" s="1"/>
+      <c r="GY10" s="4" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:203" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:208" x14ac:dyDescent="0.2">
       <c r="B11" s="9" t="s">
         <v>23</v>
       </c>
@@ -2042,26 +2066,26 @@
       <c r="BU11" s="25"/>
       <c r="DL11" s="1"/>
       <c r="DO11" s="1"/>
-      <c r="DZ11" s="59" t="s">
+      <c r="DZ11" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="EA11" s="59"/>
-      <c r="EB11" s="59"/>
-      <c r="EC11" s="59"/>
-      <c r="ED11" s="59"/>
-      <c r="EE11" s="59"/>
-      <c r="EF11" s="59"/>
-      <c r="EG11" s="59"/>
-      <c r="EH11" s="59"/>
-      <c r="EI11" s="59"/>
-      <c r="EJ11" s="59"/>
-      <c r="EK11" s="59"/>
-      <c r="EL11" s="59"/>
-      <c r="EM11" s="59"/>
+      <c r="EA11" s="50"/>
+      <c r="EB11" s="50"/>
+      <c r="EC11" s="50"/>
+      <c r="ED11" s="50"/>
+      <c r="EE11" s="50"/>
+      <c r="EF11" s="50"/>
+      <c r="EG11" s="50"/>
+      <c r="EH11" s="50"/>
+      <c r="EI11" s="50"/>
+      <c r="EJ11" s="50"/>
+      <c r="EK11" s="50"/>
+      <c r="EL11" s="50"/>
+      <c r="EM11" s="50"/>
       <c r="FA11" s="1"/>
       <c r="FH11" s="1"/>
     </row>
-    <row r="12" spans="1:203" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:208" x14ac:dyDescent="0.2">
       <c r="B12" s="9" t="s">
         <v>43</v>
       </c>
@@ -2107,7 +2131,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" spans="1:203" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:208" x14ac:dyDescent="0.2">
       <c r="B13" s="9" t="s">
         <v>46</v>
       </c>
@@ -2142,22 +2166,22 @@
       <c r="AE13" s="9"/>
       <c r="AF13" s="9"/>
       <c r="BM13" s="1"/>
-      <c r="BN13" s="55" t="s">
+      <c r="BN13" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="BO13" s="55"/>
-      <c r="BP13" s="55"/>
-      <c r="BQ13" s="55"/>
-      <c r="BR13" s="55"/>
-      <c r="BS13" s="55"/>
+      <c r="BO13" s="58"/>
+      <c r="BP13" s="58"/>
+      <c r="BQ13" s="58"/>
+      <c r="BR13" s="58"/>
+      <c r="BS13" s="58"/>
       <c r="BU13" s="25"/>
-      <c r="BV13" s="58" t="s">
+      <c r="BV13" s="64" t="s">
         <v>45</v>
       </c>
-      <c r="BW13" s="55"/>
-      <c r="BX13" s="55"/>
-      <c r="BY13" s="55"/>
-      <c r="BZ13" s="55"/>
+      <c r="BW13" s="58"/>
+      <c r="BX13" s="58"/>
+      <c r="BY13" s="58"/>
+      <c r="BZ13" s="58"/>
       <c r="DL13" s="1"/>
       <c r="DO13" s="1"/>
       <c r="EA13" s="1"/>
@@ -2165,7 +2189,7 @@
       <c r="FA13" s="1"/>
       <c r="FH13" s="1"/>
     </row>
-    <row r="14" spans="1:203" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:208" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B14" s="9" t="s">
         <v>47</v>
       </c>
@@ -2202,15 +2226,15 @@
       <c r="AG14" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="BD14" s="67" t="s">
+      <c r="BD14" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="BE14" s="67"/>
-      <c r="BF14" s="67"/>
-      <c r="BG14" s="67"/>
-      <c r="BH14" s="67"/>
-      <c r="BI14" s="67"/>
-      <c r="BJ14" s="67"/>
+      <c r="BE14" s="59"/>
+      <c r="BF14" s="59"/>
+      <c r="BG14" s="59"/>
+      <c r="BH14" s="59"/>
+      <c r="BI14" s="59"/>
+      <c r="BJ14" s="59"/>
       <c r="BM14" s="44" t="s">
         <v>59</v>
       </c>
@@ -2218,10 +2242,10 @@
       <c r="BV14" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="DD14" s="53" t="s">
+      <c r="DD14" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="DE14" s="53"/>
+      <c r="DE14" s="69"/>
       <c r="DF14" s="40"/>
       <c r="DG14" s="46"/>
       <c r="DH14" s="46"/>
@@ -2245,10 +2269,10 @@
       <c r="DV14" s="46"/>
       <c r="DW14" s="46"/>
       <c r="DX14" s="46"/>
-      <c r="DY14" s="51" t="s">
+      <c r="DY14" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="DZ14" s="52"/>
+      <c r="DZ14" s="68"/>
       <c r="EA14" s="37" t="s">
         <v>60</v>
       </c>
@@ -2267,10 +2291,10 @@
       <c r="EL14" s="41"/>
       <c r="EM14" s="41"/>
       <c r="EN14" s="41"/>
-      <c r="EO14" s="54" t="s">
+      <c r="EO14" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="EP14" s="54"/>
+      <c r="EP14" s="70"/>
       <c r="EQ14" s="48"/>
       <c r="ER14" s="48"/>
       <c r="ES14" s="48"/>
@@ -2296,25 +2320,25 @@
       <c r="FI14" s="48"/>
       <c r="FJ14" s="48"/>
     </row>
-    <row r="15" spans="1:203" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:203" x14ac:dyDescent="0.2">
-      <c r="B16" s="57" t="s">
+    <row r="15" spans="1:208" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:208" x14ac:dyDescent="0.2">
+      <c r="B16" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="69" t="s">
+      <c r="C16" s="60" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="69"/>
-      <c r="I16" s="69"/>
-      <c r="J16" s="69"/>
-      <c r="K16" s="69"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="69"/>
-      <c r="N16" s="69"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="60"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
+      <c r="N16" s="60"/>
       <c r="O16" s="20"/>
       <c r="P16" s="20"/>
       <c r="Q16" s="20"/>
@@ -2336,30 +2360,30 @@
       <c r="BD16" s="31"/>
       <c r="BE16" s="31"/>
       <c r="BF16" s="31"/>
-      <c r="BG16" s="64" t="s">
+      <c r="BG16" s="55" t="s">
         <v>66</v>
       </c>
-      <c r="BH16" s="65"/>
-      <c r="BI16" s="65"/>
-      <c r="BJ16" s="65"/>
-      <c r="BK16" s="66"/>
+      <c r="BH16" s="56"/>
+      <c r="BI16" s="56"/>
+      <c r="BJ16" s="56"/>
+      <c r="BK16" s="57"/>
     </row>
-    <row r="17" spans="1:203" x14ac:dyDescent="0.2">
-      <c r="B17" s="57"/>
-      <c r="C17" s="69" t="s">
+    <row r="17" spans="1:208" x14ac:dyDescent="0.2">
+      <c r="B17" s="63"/>
+      <c r="C17" s="60" t="s">
         <v>68</v>
       </c>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="69"/>
-      <c r="I17" s="69"/>
-      <c r="J17" s="69"/>
-      <c r="K17" s="69"/>
-      <c r="L17" s="69"/>
-      <c r="M17" s="69"/>
-      <c r="N17" s="69"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="60"/>
+      <c r="K17" s="60"/>
+      <c r="L17" s="60"/>
+      <c r="M17" s="60"/>
+      <c r="N17" s="60"/>
       <c r="O17" s="20"/>
       <c r="P17" s="20"/>
       <c r="Q17" s="20"/>
@@ -2381,13 +2405,13 @@
       <c r="BD17" s="31"/>
       <c r="BE17" s="31"/>
       <c r="BF17" s="31"/>
-      <c r="BG17" s="64" t="s">
+      <c r="BG17" s="55" t="s">
         <v>65</v>
       </c>
-      <c r="BH17" s="65"/>
-      <c r="BI17" s="65"/>
-      <c r="BJ17" s="65"/>
-      <c r="BK17" s="66"/>
+      <c r="BH17" s="56"/>
+      <c r="BI17" s="56"/>
+      <c r="BJ17" s="56"/>
+      <c r="BK17" s="57"/>
       <c r="DA17" s="1" t="s">
         <v>12</v>
       </c>
@@ -2398,8 +2422,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:203" x14ac:dyDescent="0.2">
-      <c r="B18" s="57"/>
+    <row r="18" spans="1:208" x14ac:dyDescent="0.2">
+      <c r="B18" s="63"/>
       <c r="C18" s="20"/>
       <c r="D18" s="20"/>
       <c r="E18" s="20"/>
@@ -2442,11 +2466,11 @@
       <c r="DP18" s="1"/>
       <c r="DT18" s="1"/>
     </row>
-    <row r="19" spans="1:203" x14ac:dyDescent="0.2">
-      <c r="A19" s="60" t="s">
+    <row r="19" spans="1:208" x14ac:dyDescent="0.2">
+      <c r="A19" s="51" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="62"/>
+      <c r="B19" s="53"/>
       <c r="C19" s="16">
         <v>43843</v>
       </c>
@@ -3050,8 +3074,23 @@
       <c r="GU19" s="17">
         <v>44043</v>
       </c>
+      <c r="GV19" s="17">
+        <v>44044</v>
+      </c>
+      <c r="GW19" s="17">
+        <v>44045</v>
+      </c>
+      <c r="GX19" s="17">
+        <v>44046</v>
+      </c>
+      <c r="GY19" s="17">
+        <v>44047</v>
+      </c>
+      <c r="GZ19" s="17">
+        <v>44048</v>
+      </c>
     </row>
-    <row r="20" spans="1:203" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:208" x14ac:dyDescent="0.2">
       <c r="B20" s="9" t="s">
         <v>17</v>
       </c>
@@ -3111,7 +3150,7 @@
       <c r="FA20" s="1"/>
       <c r="FH20" s="1"/>
     </row>
-    <row r="21" spans="1:203" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:208" x14ac:dyDescent="0.2">
       <c r="B21" s="9" t="s">
         <v>22</v>
       </c>
@@ -3165,7 +3204,7 @@
       <c r="FA21" s="1"/>
       <c r="FH21" s="1"/>
     </row>
-    <row r="22" spans="1:203" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:208" x14ac:dyDescent="0.2">
       <c r="B22" s="9" t="s">
         <v>46</v>
       </c>
@@ -3208,28 +3247,28 @@
       <c r="BJ22" s="31"/>
       <c r="BK22" s="31"/>
       <c r="BM22" s="1"/>
-      <c r="BN22" s="55" t="s">
+      <c r="BN22" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="BO22" s="55"/>
-      <c r="BP22" s="55"/>
-      <c r="BQ22" s="55"/>
-      <c r="BR22" s="55"/>
-      <c r="BS22" s="55"/>
-      <c r="BV22" s="55" t="s">
+      <c r="BO22" s="58"/>
+      <c r="BP22" s="58"/>
+      <c r="BQ22" s="58"/>
+      <c r="BR22" s="58"/>
+      <c r="BS22" s="58"/>
+      <c r="BV22" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="BW22" s="55"/>
-      <c r="BX22" s="55"/>
-      <c r="BY22" s="55"/>
-      <c r="BZ22" s="55"/>
+      <c r="BW22" s="58"/>
+      <c r="BX22" s="58"/>
+      <c r="BY22" s="58"/>
+      <c r="BZ22" s="58"/>
       <c r="DL22" s="1"/>
       <c r="DO22" s="1"/>
       <c r="EA22" s="1"/>
       <c r="FA22" s="1"/>
       <c r="FH22" s="1"/>
     </row>
-    <row r="23" spans="1:203" s="42" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:208" s="42" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B23" s="9" t="s">
         <v>47</v>
       </c>
@@ -3266,15 +3305,15 @@
       <c r="AG23" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="BD23" s="67" t="s">
+      <c r="BD23" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="BE23" s="67"/>
-      <c r="BF23" s="67"/>
-      <c r="BG23" s="67"/>
-      <c r="BH23" s="67"/>
-      <c r="BI23" s="67"/>
-      <c r="BJ23" s="67"/>
+      <c r="BE23" s="59"/>
+      <c r="BF23" s="59"/>
+      <c r="BG23" s="59"/>
+      <c r="BH23" s="59"/>
+      <c r="BI23" s="59"/>
+      <c r="BJ23" s="59"/>
       <c r="BM23" s="44" t="s">
         <v>59</v>
       </c>
@@ -3282,10 +3321,10 @@
       <c r="BV23" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="DD23" s="53" t="s">
+      <c r="DD23" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="DE23" s="53"/>
+      <c r="DE23" s="69"/>
       <c r="DF23" s="40"/>
       <c r="DG23" s="46"/>
       <c r="DH23" s="46"/>
@@ -3309,10 +3348,10 @@
       <c r="DV23" s="46"/>
       <c r="DW23" s="46"/>
       <c r="DX23" s="46"/>
-      <c r="DY23" s="51" t="s">
+      <c r="DY23" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="DZ23" s="52"/>
+      <c r="DZ23" s="68"/>
       <c r="EA23" s="37" t="s">
         <v>60</v>
       </c>
@@ -3331,10 +3370,10 @@
       <c r="EL23" s="41"/>
       <c r="EM23" s="41"/>
       <c r="EN23" s="41"/>
-      <c r="EO23" s="54" t="s">
+      <c r="EO23" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="EP23" s="54"/>
+      <c r="EP23" s="70"/>
       <c r="EQ23" s="48"/>
       <c r="ER23" s="48"/>
       <c r="ES23" s="48"/>
@@ -3360,7 +3399,7 @@
       <c r="FI23" s="48"/>
       <c r="FJ23" s="48"/>
     </row>
-    <row r="24" spans="1:203" s="15" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:208" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="BD24" s="32"/>
       <c r="BE24" s="32"/>
       <c r="BF24" s="32"/>
@@ -3370,7 +3409,7 @@
       <c r="BJ24" s="32"/>
       <c r="BK24" s="32"/>
     </row>
-    <row r="25" spans="1:203" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:208" x14ac:dyDescent="0.2">
       <c r="BD25" s="31"/>
       <c r="BE25" s="31"/>
       <c r="BF25" s="31"/>
@@ -3380,7 +3419,7 @@
       <c r="BJ25" s="31"/>
       <c r="BK25" s="31"/>
     </row>
-    <row r="26" spans="1:203" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:208" x14ac:dyDescent="0.2">
       <c r="BD26" s="31"/>
       <c r="BE26" s="31"/>
       <c r="BF26" s="31"/>
@@ -3390,24 +3429,24 @@
       <c r="BJ26" s="31"/>
       <c r="BK26" s="31"/>
     </row>
-    <row r="27" spans="1:203" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:208" x14ac:dyDescent="0.2">
       <c r="B27" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="70" t="s">
+      <c r="C27" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="D27" s="70"/>
-      <c r="E27" s="70"/>
-      <c r="F27" s="70"/>
-      <c r="G27" s="70"/>
-      <c r="H27" s="70"/>
-      <c r="I27" s="70"/>
-      <c r="J27" s="70"/>
-      <c r="K27" s="70"/>
-      <c r="L27" s="70"/>
-      <c r="M27" s="70"/>
-      <c r="N27" s="70"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="61"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="61"/>
+      <c r="L27" s="61"/>
+      <c r="M27" s="61"/>
+      <c r="N27" s="61"/>
       <c r="O27" s="36"/>
       <c r="P27" s="36"/>
       <c r="Q27" s="36"/>
@@ -3426,13 +3465,13 @@
       <c r="BD27" s="31"/>
       <c r="BE27" s="31"/>
       <c r="BF27" s="31"/>
-      <c r="BG27" s="64" t="s">
+      <c r="BG27" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="BH27" s="65"/>
-      <c r="BI27" s="65"/>
-      <c r="BJ27" s="65"/>
-      <c r="BK27" s="66"/>
+      <c r="BH27" s="56"/>
+      <c r="BI27" s="56"/>
+      <c r="BJ27" s="56"/>
+      <c r="BK27" s="57"/>
       <c r="EN27" s="1" t="s">
         <v>30</v>
       </c>
@@ -3452,24 +3491,24 @@
         <v>39</v>
       </c>
     </row>
-    <row r="28" spans="1:203" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:208" x14ac:dyDescent="0.2">
       <c r="B28" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="C28" s="70" t="s">
+      <c r="C28" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="70"/>
-      <c r="E28" s="70"/>
-      <c r="F28" s="70"/>
-      <c r="G28" s="70"/>
-      <c r="H28" s="70"/>
-      <c r="I28" s="70"/>
-      <c r="J28" s="70"/>
-      <c r="K28" s="70"/>
-      <c r="L28" s="70"/>
-      <c r="M28" s="70"/>
-      <c r="N28" s="70"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="61"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="61"/>
+      <c r="K28" s="61"/>
+      <c r="L28" s="61"/>
+      <c r="M28" s="61"/>
+      <c r="N28" s="61"/>
       <c r="O28" s="36"/>
       <c r="P28" s="36"/>
       <c r="Q28" s="36"/>
@@ -3488,13 +3527,13 @@
       <c r="BD28" s="31"/>
       <c r="BE28" s="31"/>
       <c r="BF28" s="31"/>
-      <c r="BG28" s="64" t="s">
+      <c r="BG28" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="BH28" s="65"/>
-      <c r="BI28" s="65"/>
-      <c r="BJ28" s="65"/>
-      <c r="BK28" s="66"/>
+      <c r="BH28" s="56"/>
+      <c r="BI28" s="56"/>
+      <c r="BJ28" s="56"/>
+      <c r="BK28" s="57"/>
       <c r="DQ28" s="1" t="s">
         <v>27</v>
       </c>
@@ -3507,7 +3546,7 @@
       <c r="EX28" s="1"/>
       <c r="FA28" s="1"/>
     </row>
-    <row r="29" spans="1:203" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:208" x14ac:dyDescent="0.2">
       <c r="DQ29" s="1"/>
       <c r="EN29" s="1"/>
       <c r="ER29" s="1"/>
@@ -3516,11 +3555,11 @@
       <c r="EX29" s="1"/>
       <c r="FA29" s="1"/>
     </row>
-    <row r="30" spans="1:203" x14ac:dyDescent="0.2">
-      <c r="A30" s="60" t="s">
+    <row r="30" spans="1:208" x14ac:dyDescent="0.2">
+      <c r="A30" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="B30" s="60"/>
+      <c r="B30" s="51"/>
       <c r="C30" s="16">
         <v>43843</v>
       </c>
@@ -4124,8 +4163,23 @@
       <c r="GU30" s="17">
         <v>44043</v>
       </c>
+      <c r="GV30" s="17">
+        <v>44044</v>
+      </c>
+      <c r="GW30" s="17">
+        <v>44045</v>
+      </c>
+      <c r="GX30" s="17">
+        <v>44046</v>
+      </c>
+      <c r="GY30" s="17">
+        <v>44047</v>
+      </c>
+      <c r="GZ30" s="17">
+        <v>44048</v>
+      </c>
     </row>
-    <row r="31" spans="1:203" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:208" x14ac:dyDescent="0.2">
       <c r="B31" s="9" t="s">
         <v>17</v>
       </c>
@@ -4175,7 +4229,7 @@
       <c r="FA31" s="1"/>
       <c r="FH31" s="1"/>
     </row>
-    <row r="32" spans="1:203" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:208" x14ac:dyDescent="0.2">
       <c r="B32" s="9" t="s">
         <v>22</v>
       </c>
@@ -4270,21 +4324,21 @@
       <c r="AE33" s="9"/>
       <c r="AF33" s="9"/>
       <c r="BM33" s="1"/>
-      <c r="BN33" s="55" t="s">
+      <c r="BN33" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="BO33" s="55"/>
-      <c r="BP33" s="55"/>
-      <c r="BQ33" s="55"/>
-      <c r="BR33" s="55"/>
-      <c r="BS33" s="55"/>
-      <c r="BV33" s="55" t="s">
+      <c r="BO33" s="58"/>
+      <c r="BP33" s="58"/>
+      <c r="BQ33" s="58"/>
+      <c r="BR33" s="58"/>
+      <c r="BS33" s="58"/>
+      <c r="BV33" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="BW33" s="55"/>
-      <c r="BX33" s="55"/>
-      <c r="BY33" s="55"/>
-      <c r="BZ33" s="55"/>
+      <c r="BW33" s="58"/>
+      <c r="BX33" s="58"/>
+      <c r="BY33" s="58"/>
+      <c r="BZ33" s="58"/>
       <c r="DL33" s="1"/>
       <c r="DO33" s="1"/>
       <c r="EA33" s="1"/>
@@ -4328,15 +4382,15 @@
       <c r="AG34" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="BD34" s="67" t="s">
+      <c r="BD34" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="BE34" s="67"/>
-      <c r="BF34" s="67"/>
-      <c r="BG34" s="67"/>
-      <c r="BH34" s="67"/>
-      <c r="BI34" s="67"/>
-      <c r="BJ34" s="67"/>
+      <c r="BE34" s="59"/>
+      <c r="BF34" s="59"/>
+      <c r="BG34" s="59"/>
+      <c r="BH34" s="59"/>
+      <c r="BI34" s="59"/>
+      <c r="BJ34" s="59"/>
       <c r="BM34" s="44" t="s">
         <v>59</v>
       </c>
@@ -4344,10 +4398,10 @@
       <c r="BV34" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="DD34" s="53" t="s">
+      <c r="DD34" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="DE34" s="53"/>
+      <c r="DE34" s="69"/>
       <c r="DF34" s="40"/>
       <c r="DG34" s="46"/>
       <c r="DH34" s="46"/>
@@ -4371,10 +4425,10 @@
       <c r="DV34" s="46"/>
       <c r="DW34" s="46"/>
       <c r="DX34" s="46"/>
-      <c r="DY34" s="51" t="s">
+      <c r="DY34" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="DZ34" s="52"/>
+      <c r="DZ34" s="68"/>
       <c r="EA34" s="37" t="s">
         <v>60</v>
       </c>
@@ -4393,10 +4447,10 @@
       <c r="EL34" s="41"/>
       <c r="EM34" s="41"/>
       <c r="EN34" s="41"/>
-      <c r="EO34" s="54" t="s">
+      <c r="EO34" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="EP34" s="54"/>
+      <c r="EP34" s="70"/>
       <c r="EQ34" s="48"/>
       <c r="ER34" s="48"/>
       <c r="ES34" s="48"/>
@@ -4424,10 +4478,10 @@
     </row>
     <row r="35" spans="1:166" s="15" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:166" x14ac:dyDescent="0.2">
-      <c r="A37" s="50" t="s">
+      <c r="A37" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="50"/>
+      <c r="B37" s="66"/>
     </row>
     <row r="38" spans="1:166" x14ac:dyDescent="0.2">
       <c r="A38" s="21"/>
@@ -4507,6 +4561,25 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="DY14:DZ14"/>
+    <mergeCell ref="DD14:DE14"/>
+    <mergeCell ref="EO14:EP14"/>
+    <mergeCell ref="DD23:DE23"/>
+    <mergeCell ref="DY23:DZ23"/>
+    <mergeCell ref="EO23:EP23"/>
+    <mergeCell ref="DD34:DE34"/>
+    <mergeCell ref="DY34:DZ34"/>
+    <mergeCell ref="EO34:EP34"/>
+    <mergeCell ref="BV33:BZ33"/>
+    <mergeCell ref="BN33:BS33"/>
+    <mergeCell ref="BD34:BJ34"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="BN13:BS13"/>
+    <mergeCell ref="BV13:BZ13"/>
+    <mergeCell ref="BN22:BS22"/>
+    <mergeCell ref="C6:N6"/>
     <mergeCell ref="DZ11:EM11"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A19:B19"/>
@@ -4523,25 +4596,6 @@
     <mergeCell ref="C16:N16"/>
     <mergeCell ref="C28:N28"/>
     <mergeCell ref="C27:N27"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="BN13:BS13"/>
-    <mergeCell ref="BV13:BZ13"/>
-    <mergeCell ref="BN22:BS22"/>
-    <mergeCell ref="C6:N6"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="DY14:DZ14"/>
-    <mergeCell ref="DD14:DE14"/>
-    <mergeCell ref="EO14:EP14"/>
-    <mergeCell ref="DD23:DE23"/>
-    <mergeCell ref="DY23:DZ23"/>
-    <mergeCell ref="EO23:EP23"/>
-    <mergeCell ref="DD34:DE34"/>
-    <mergeCell ref="DY34:DZ34"/>
-    <mergeCell ref="EO34:EP34"/>
-    <mergeCell ref="BV33:BZ33"/>
-    <mergeCell ref="BN33:BS33"/>
-    <mergeCell ref="BD34:BJ34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>